<commit_message>
CR- EITL is to modified for Implementation of all featured
</commit_message>
<xml_diff>
--- a/App_Templates/IW_Template.xlsx
+++ b/App_Templates/IW_Template.xlsx
@@ -696,6 +696,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -740,14 +748,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1116,7 +1116,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1145,13 +1145,13 @@
     <row r="2" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="45"/>
       <c r="B2" s="46"/>
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="64"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="66"/>
     </row>
     <row r="3" spans="1:7" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A3" s="47"/>
@@ -1160,10 +1160,10 @@
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="66"/>
+      <c r="F3" s="68"/>
       <c r="G3" s="48"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1173,10 +1173,10 @@
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="67" t="s">
+      <c r="E4" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="68"/>
+      <c r="F4" s="70"/>
       <c r="G4" s="49"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1186,10 +1186,10 @@
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="67" t="s">
+      <c r="E5" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="68"/>
+      <c r="F5" s="70"/>
       <c r="G5" s="50"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1199,8 +1199,8 @@
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="68"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="70"/>
       <c r="G6" s="49"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1210,10 +1210,10 @@
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="67" t="s">
+      <c r="E7" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="68"/>
+      <c r="F7" s="70"/>
       <c r="G7" s="49"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1223,10 +1223,10 @@
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="67" t="s">
+      <c r="E8" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="68"/>
+      <c r="F8" s="70"/>
       <c r="G8" s="49"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1236,10 +1236,10 @@
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="67" t="s">
+      <c r="E9" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="68"/>
+      <c r="F9" s="70"/>
       <c r="G9" s="49"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1249,8 +1249,8 @@
       </c>
       <c r="C10" s="53"/>
       <c r="D10" s="54"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="70"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="72"/>
       <c r="G10" s="55"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1305,25 +1305,25 @@
     </row>
     <row r="15" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="31"/>
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="58"/>
-      <c r="G15" s="59"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="61"/>
     </row>
     <row r="16" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="32"/>
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="61"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="63"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="31"/>
@@ -1349,8 +1349,8 @@
       <c r="C19" s="12"/>
       <c r="D19" s="25"/>
       <c r="E19" s="25"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="72"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="57"/>
     </row>
     <row r="20" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="32"/>
@@ -1358,8 +1358,8 @@
       <c r="C20" s="26"/>
       <c r="D20" s="25"/>
       <c r="E20" s="25"/>
-      <c r="F20" s="71"/>
-      <c r="G20" s="72"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="57"/>
     </row>
     <row r="21" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="32"/>
@@ -1371,10 +1371,10 @@
       </c>
       <c r="D21" s="28"/>
       <c r="E21" s="28"/>
-      <c r="F21" s="56" t="s">
+      <c r="F21" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="G21" s="57"/>
+      <c r="G21" s="59"/>
     </row>
     <row r="22" spans="1:7" ht="1.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="35"/>
@@ -1386,7 +1386,7 @@
       <c r="G22" s="39"/>
     </row>
   </sheetData>
-  <sheetProtection password="CF0D" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" autoFilter="0"/>
+  <sheetProtection password="CF0D" sheet="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" autoFilter="0"/>
   <mergeCells count="12">
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="B15:G15"/>

</xml_diff>